<commit_message>
Update Section 4 analysis scripts and Excel files
- Refactored q26.py and q27.py to streamline data analysis by utilizing a shared utility function for running analyses.
- Removed redundant code and improved clarity in the scripts.
- Updated Excel files in Section 4 to ensure they reflect the latest survey data on OWASP API security risks and organizational readiness.
- Deleted trial.py as it was no longer needed.
</commit_message>
<xml_diff>
--- a/data/Section4/27 How ready is your organization in mitigating these risks.xlsx
+++ b/data/Section4/27 How ready is your organization in mitigating these risks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Survey Report Agent/surveyreport/data/Section 4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorgft15392477-my.sharepoint.com/personal/nitin_acharekar_smartvalyou_ai/Documents/Survey Report/Survey Report Agent/surveyreport/data/Section4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{ED1A6C35-8CC8-4D51-B8ED-D4CB36CA6AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3797C11D-9FC0-4252-9093-547492FBC061}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{ED1A6C35-8CC8-4D51-B8ED-D4CB36CA6AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8BEA81B-EFE9-41DC-9710-0ABEF89E35D5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBE9570F-DD10-4F10-B1E1-3F9C3143E800}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DBE9570F-DD10-4F10-B1E1-3F9C3143E800}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4036" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4038" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Count of API2:2023 - Broken Authentication</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -18510,6 +18516,17 @@
     </ext>
   </extLst>
 </pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0B29CBB7-3708-484D-A398-F1CC77F65FFC}" name="Table1" displayName="Table1" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{0B29CBB7-3708-484D-A398-F1CC77F65FFC}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{B200D90C-E810-47E0-B629-6DDB168DDDDF}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{9DD50605-8122-4DAA-8944-C243C790186F}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18831,7 +18848,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C988D53F-DE77-479B-9DA9-CEBA1FA6A0BD}">
   <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -68899,10 +68916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E1F246-8E60-4436-A257-217537A4D3F5}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68912,55 +68929,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
+      <c r="A1" t="s">
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -69313,11 +69341,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc48c5df-3b0f-414f-aba8-6581fa801985" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69554,27 +69583,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc48c5df-3b0f-414f-aba8-6581fa801985" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD2B125B-3A82-413F-A90C-B66AE31B1C84}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FB2BC5E-E378-45DA-AD7F-FB3C649961DC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7c288d03-abb0-40cb-a891-02024b2e663f"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="dc48c5df-3b0f-414f-aba8-6581fa801985"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -69599,9 +69618,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FB2BC5E-E378-45DA-AD7F-FB3C649961DC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD2B125B-3A82-413F-A90C-B66AE31B1C84}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7c288d03-abb0-40cb-a891-02024b2e663f"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="dc48c5df-3b0f-414f-aba8-6581fa801985"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>